<commit_message>
Upadated for excel template about add ID column
</commit_message>
<xml_diff>
--- a/static/sample.xlsx
+++ b/static/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\vcard\vcard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jameshyt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAAD970-90E4-4344-AAEF-2091B5396F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9686E875-CAF9-479D-9EF6-C2B252301DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5552708-718E-4AFD-B796-56BBD3A27C93}"/>
   </bookViews>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>family_name</t>
-  </si>
-  <si>
-    <t>given_name</t>
-  </si>
-  <si>
-    <t>full_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>email</t>
   </si>
@@ -60,31 +51,49 @@
     <t>website</t>
   </si>
   <si>
-    <t>Hu</t>
-  </si>
-  <si>
-    <t>James Hu</t>
-  </si>
-  <si>
-    <t>jameshu@xensetech.hk</t>
-  </si>
-  <si>
-    <t>www.xensetech.hk</t>
-  </si>
-  <si>
-    <t>Tam</t>
-  </si>
-  <si>
-    <t>Johnny Tam</t>
-  </si>
-  <si>
-    <t>C.H. Johnny</t>
-  </si>
-  <si>
-    <t>Y.T. James</t>
-  </si>
-  <si>
-    <t>johnnytam@xensetech.hk</t>
+    <t>title</t>
+  </si>
+  <si>
+    <t>direct_line</t>
+  </si>
+  <si>
+    <t>staff_id</t>
+  </si>
+  <si>
+    <t>www.pyengineering.com</t>
+  </si>
+  <si>
+    <t>anotherone@pyengineering.com</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>00002</t>
+  </si>
+  <si>
+    <t>Sample Guy</t>
+  </si>
+  <si>
+    <t>jameshu@pyengineering.com</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>28383030</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>James Y.T. Hu</t>
+  </si>
+  <si>
+    <t>John N.B. Doe</t>
   </si>
 </sst>
 </file>
@@ -131,9 +140,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -449,95 +459,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BCB4E4-F01A-47EA-8EAC-FF7A62431F5C}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>12345600</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>28383030</v>
-      </c>
-      <c r="F2">
-        <v>65612892</v>
-      </c>
-      <c r="G2">
-        <v>65612892</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" s="1">
+        <v>28282828</v>
+      </c>
+      <c r="D3" s="1">
+        <v>65656565</v>
+      </c>
+      <c r="E3" s="1">
+        <v>12345600</v>
+      </c>
+      <c r="F3" s="1">
+        <v>12348765</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>28383048</v>
-      </c>
-      <c r="F3">
-        <v>62760183</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{AD6DA03B-2A99-4C04-9941-E6A48E86EE4D}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{26610311-9A99-4701-B0C1-66A4824B5242}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{663E9C07-E364-47F6-9E07-C9599EADD2C7}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{0B0FC2BF-7570-4860-92A2-A1F98FFE32A2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AD6DA03B-2A99-4C04-9941-E6A48E86EE4D}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{26610311-9A99-4701-B0C1-66A4824B5242}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{BBB783FB-6EDE-4E95-B138-3EB601937C4A}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{8690B5BD-E723-4A8E-A9DB-336434E15317}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>

</xml_diff>